<commit_message>
Implemented reconcile applications for addVisitorForExisting Individual class.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="addVisitor" r:id="rId2" sheetId="1" state="visible"/>
-    <sheet name="sqlCount" r:id="rId3" sheetId="2" state="visible"/>
+    <sheet name="addBrandNewVisitor" r:id="rId2" sheetId="1" state="visible"/>
+    <sheet name="addVisitorForExistingIndividual" r:id="rId3" sheetId="2" state="visible"/>
+    <sheet name="sqlCount" r:id="rId4" sheetId="3" state="visible"/>
   </sheets>
   <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
   <extLst>
@@ -21,27 +22,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve">brandNewVisitorEmailId</t>
   </si>
   <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SeleniumTest+v20191112113007@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test+v20191112113007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SeleniumTest+v20191112113325@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test+v20191112113325</t>
+  </si>
+  <si>
     <t xml:space="preserve">sqlRecordCount</t>
   </si>
   <si>
     <t xml:space="preserve">sqlColCount</t>
   </si>
   <si>
-    <t>SeleniumTest+v20191017153943@gmail.com</t>
-  </si>
-  <si>
-    <t>SeleniumTest+v20191017154305@gmail.com</t>
-  </si>
-  <si>
-    <t>252</t>
-  </si>
-  <si>
-    <t>5</t>
+    <t xml:space="preserve">252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t>Test20191113101536</t>
+  </si>
+  <si>
+    <t>Test+v20191113102017</t>
+  </si>
+  <si>
+    <t>Test+v20191113104808</t>
+  </si>
+  <si>
+    <t>Test+v20191113105421</t>
+  </si>
+  <si>
+    <t>Test+v20191113110438</t>
   </si>
 </sst>
 </file>
@@ -138,15 +163,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="20.6" collapsed="true" outlineLevel="0"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="38.39" collapsed="true" outlineLevel="0"/>
     <col min="2" max="2" customWidth="true" hidden="false" style="0" width="14.35" collapsed="true" outlineLevel="0"/>
     <col min="3" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
@@ -155,15 +180,24 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
         <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -178,6 +212,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="14.35" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -196,18 +266,18 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included feature files, pageobjects and java classes for online renewals.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -2,17 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" date1904="false" showObjects="all"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="addBrandNewVisitor" r:id="rId2" sheetId="1" state="visible"/>
-    <sheet name="addVisitorForExistingIndividual" r:id="rId3" sheetId="2" state="visible"/>
-    <sheet name="sqlCount" r:id="rId4" sheetId="3" state="visible"/>
+    <sheet name="addBrandNewVisitor" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="addVisitorForExistingIndividual" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="sqlCount" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t xml:space="preserve">brandNewVisitorEmailId</t>
   </si>
@@ -52,21 +52,6 @@
   </si>
   <si>
     <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t>Test20191113101536</t>
-  </si>
-  <si>
-    <t>Test+v20191113102017</t>
-  </si>
-  <si>
-    <t>Test+v20191113104808</t>
-  </si>
-  <si>
-    <t>Test+v20191113105421</t>
-  </si>
-  <si>
-    <t>Test+v20191113110438</t>
   </si>
 </sst>
 </file>
@@ -108,7 +93,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -117,43 +102,43 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -163,20 +148,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="38.39" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="14.35" collapsed="true" outlineLevel="0"/>
-    <col min="3" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -184,7 +169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
@@ -192,7 +177,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
@@ -201,9 +186,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -216,30 +201,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="14.35" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -252,19 +235,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="14.35" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>6</v>
       </c>
@@ -272,7 +255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
@@ -281,9 +264,9 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
'EventRegistrationForAMember' feature completed. This commit includes features files, page objects and steps for this feature.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="addBrandNewVisitor" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="addVisitorForExistingIndividual" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="sqlCount" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="createRegionalEvent" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="sqlCount" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,12 +23,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t xml:space="preserve">brandNewVisitorEmailId</t>
   </si>
   <si>
     <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eventName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestAutomation20191204134548</t>
   </si>
   <si>
     <t xml:space="preserve">sqlRecordCount</t>
@@ -138,7 +145,7 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -175,7 +182,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -207,6 +214,44 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -221,18 +266,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
'amendStatusOfNonMemberViaDueDate' feature completed(verification part TBC, will be covered in a separate feature file)
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="addBrandNewVisitor" r:id="rId2" sheetId="1" state="visible"/>
     <sheet name="addVisitorForExistingIndividual" r:id="rId3" sheetId="2" state="visible"/>
     <sheet name="createRegionalEvent" r:id="rId4" sheetId="3" state="visible"/>
-    <sheet name="sqlCount" r:id="rId5" sheetId="4" state="visible"/>
+    <sheet name="amendStatusOfNonMemberViaDueDate" r:id="rId5" sheetId="4" state="visible"/>
+    <sheet name="sqlCount" r:id="rId6" sheetId="5" state="visible"/>
   </sheets>
   <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t xml:space="preserve">brandNewVisitorEmailId</t>
   </si>
@@ -34,6 +35,12 @@
     <t xml:space="preserve">eventName</t>
   </si>
   <si>
+    <t xml:space="preserve">TestAutomation20191211060135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emailId</t>
+  </si>
+  <si>
     <t xml:space="preserve">sqlRecordCount</t>
   </si>
   <si>
@@ -46,7 +53,7 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t>TestAutomation20191211060135</t>
+    <t>shanthibni+32@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -145,7 +152,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -216,7 +223,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -231,23 +238,60 @@
         <v>2</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <cols>
+    <col min="1" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -266,18 +310,18 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in requirement hence code and feature files are changed (palms)
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t xml:space="preserve">brandNewVisitorEmailId</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>shanthibni+32@gmail.com</t>
+  </si>
+  <si>
+    <t>TestAutomation20191217141856</t>
+  </si>
+  <si>
+    <t>TestAutomation20191217142208</t>
   </si>
 </sst>
 </file>
@@ -221,7 +227,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -243,6 +249,16 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>

</xml_diff>

<commit_message>
minor defect fix in DbXlsComparator.java
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="16">
   <si>
     <t xml:space="preserve">brandNewVisitorEmailId</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>252</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -340,10 +346,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included code for deleting rows in testInput.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="addBrandNewVisitor" r:id="rId2" sheetId="1" state="visible"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t xml:space="preserve">brandNewVisitorEmailId</t>
   </si>
@@ -33,12 +33,33 @@
     <t xml:space="preserve">lastName</t>
   </si>
   <si>
+    <t xml:space="preserve">g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
     <t xml:space="preserve">EmailID</t>
   </si>
   <si>
     <t xml:space="preserve">last name</t>
   </si>
   <si>
+    <t xml:space="preserve">Automationuser20200124111102@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user20200124111102</t>
+  </si>
+  <si>
     <t xml:space="preserve">eventName</t>
   </si>
   <si>
@@ -67,12 +88,6 @@
   </si>
   <si>
     <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t>Automationuser20200124111102@gmail.com</t>
-  </si>
-  <si>
-    <t>user20200124111102</t>
   </si>
 </sst>
 </file>
@@ -171,7 +186,7 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -208,7 +223,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -221,18 +236,18 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -299,94 +314,6 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
-  <cols>
-    <col min="1" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
-  </cols>
-  <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="14.35" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
-  </cols>
-  <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="0" t="s">
         <v>11</v>
       </c>
     </row>
@@ -394,8 +321,96 @@
       <c r="A2" s="0" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+      <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <cols>
+    <col min="1" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="14.35" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor defect fix(Duplicate login) in all selected files.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t xml:space="preserve">brandNewVisitorEmailId</t>
   </si>
@@ -88,6 +88,30 @@
   </si>
   <si>
     <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t>SeleniumTest+v20200128111742@gmail.com</t>
+  </si>
+  <si>
+    <t>Test+v20200128111742</t>
+  </si>
+  <si>
+    <t>SeleniumTest+v20200128112147@gmail.com</t>
+  </si>
+  <si>
+    <t>Test+v20200128112147</t>
+  </si>
+  <si>
+    <t>SeleniumTest+v20200128112937@gmail.com</t>
+  </si>
+  <si>
+    <t>Test+v20200128112937</t>
+  </si>
+  <si>
+    <t>SeleniumTest+v20200128122914@gmail.com</t>
+  </si>
+  <si>
+    <t>Test+v20200128122914</t>
   </si>
 </sst>
 </file>
@@ -184,7 +208,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -205,6 +229,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>

</xml_diff>

<commit_message>
minor code change in the GmailClient.java to accommodate comments (to parse the mail content and write it to excel) from Suresh.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -5,15 +5,17 @@
   <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="addBrandNewVisitor" r:id="rId2" sheetId="1" state="visible"/>
-    <sheet name="registerAProspectiveVisitor" r:id="rId3" sheetId="2" state="visible"/>
-    <sheet name="addVisitorForExistingIndividual" r:id="rId4" sheetId="3" state="visible"/>
-    <sheet name="createRegionalEvent" r:id="rId5" sheetId="4" state="visible"/>
-    <sheet name="amendStatusOfNonMemberViaDueDate" r:id="rId6" sheetId="5" state="visible"/>
-    <sheet name="sqlCount" r:id="rId7" sheetId="6" state="visible"/>
+    <sheet name="payment" r:id="rId2" sheetId="1" state="visible"/>
+    <sheet name="applicant" r:id="rId3" sheetId="2" state="visible"/>
+    <sheet name="addBrandNewVisitor" r:id="rId4" sheetId="3" state="visible"/>
+    <sheet name="registerAProspectiveVisitor" r:id="rId5" sheetId="4" state="visible"/>
+    <sheet name="addVisitorForExistingIndividual" r:id="rId6" sheetId="5" state="visible"/>
+    <sheet name="createRegionalEvent" r:id="rId7" sheetId="6" state="visible"/>
+    <sheet name="amendStatusOfNonMemberViaDueDate" r:id="rId8" sheetId="7" state="visible"/>
+    <sheet name="sqlCount" r:id="rId9" sheetId="8" state="visible"/>
   </sheets>
   <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
   <extLst>
@@ -25,7 +27,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+  <si>
+    <t xml:space="preserve">url</t>
+  </si>
   <si>
     <t xml:space="preserve">brandNewVisitorEmailId</t>
   </si>
@@ -33,51 +38,18 @@
     <t xml:space="preserve">lastName</t>
   </si>
   <si>
-    <t xml:space="preserve">g</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
     <t xml:space="preserve">EmailID</t>
   </si>
   <si>
     <t xml:space="preserve">last name</t>
   </si>
   <si>
-    <t xml:space="preserve">Automationuser20200124111102@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user20200124111102</t>
-  </si>
-  <si>
     <t xml:space="preserve">eventName</t>
   </si>
   <si>
-    <t xml:space="preserve">TestAutomation20191211060135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TestAutomation20191217141856</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TestAutomation20191217142208</t>
-  </si>
-  <si>
     <t xml:space="preserve">emailId</t>
   </si>
   <si>
-    <t xml:space="preserve">shanthibni+32@gmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">sqlRecordCount</t>
   </si>
   <si>
@@ -90,28 +62,10 @@
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t>SeleniumTest+v20200128111742@gmail.com</t>
-  </si>
-  <si>
-    <t>Test+v20200128111742</t>
-  </si>
-  <si>
-    <t>SeleniumTest+v20200128112147@gmail.com</t>
-  </si>
-  <si>
-    <t>Test+v20200128112147</t>
-  </si>
-  <si>
-    <t>SeleniumTest+v20200128112937@gmail.com</t>
-  </si>
-  <si>
-    <t>Test+v20200128112937</t>
-  </si>
-  <si>
-    <t>SeleniumTest+v20200128122914@gmail.com</t>
-  </si>
-  <si>
-    <t>Test+v20200128122914</t>
+    <t>https://www.bniconnectglobal.com/web/open/tokenator?concept=connect&amp;token=JFmUofFqkTdtuzjqYW3Oqtk5qlSHDIf3JMqw5JTU7r6yOU4bF4UPvaaNo2WZBuFBZBV3NCMLXdxSAnKi4wEZl%2FFIHJRdoxW%2BlY3Dw8XZjmSdbEzm1CwoGQ3JmPg75E1fA%2FRKb9vXdXo2lW2X2HEsGQsgh%2FfgoTyxvEOn4f3KyEc2MLy7zWUTpg%3D%3D&amp;chapterId=10927&amp;step=</t>
+  </si>
+  <si>
+    <t>https://www.bniconnectglobal.com/web/open/tokenator?concept=connect&amp;token=dl1fcOpOVIlwBRG70WYF%2FMbMZ183hNO3ylSHv6J0ADW4I0QFhvs7F9kXT%2BuD1SxAc%2FvQchHR9CjOYjdauFJwJgqT3bE3GH9PBOJSQo%2Bdqze4RYj5saST8kVkiOeLqyDCbQVf75YqkDzIn6jPVGw5zY7rfK05X6ZCD0f91n427Hs%3D&amp;chapterId=9406&amp;step=applicant</t>
   </si>
 </sst>
 </file>
@@ -208,9 +162,73 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <cols>
+    <col min="1" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <cols>
+    <col min="1" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -223,32 +241,24 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -268,24 +278,24 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -305,21 +315,21 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -338,21 +348,21 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -370,21 +380,21 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -403,18 +413,18 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
introduced email check in AddAndSearchBrandNewVisitor. Also changed the tags in runner class.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="payment" r:id="rId2" sheetId="1" state="visible"/>
@@ -27,9 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
-  <si>
-    <t xml:space="preserve">url</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+  <si>
+    <t xml:space="preserve">URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.bnitest2.sasyadev.com/web/open/tokenator?concept=connect&amp;token=f3K7zFEZcTG%2Becd7l%2BpcnVl%2FEQyClb0%2B2uuWO%2FIMB6X7lkCx8KShSd%2BGIKHzMfwPxDfikl4QLOHQC%2FHoi4NhEWGmvbOk1NlfQLPJFEPL5AEupitSDXlCZJcAlmnvOFQ4vPNW2iU7m9hGxslkmoqrNM8Q5%2FXOYnCN90YaChNd%2BwZ8dqv9YF2DuA%3D%3D&amp;chapterId=816&amp;step=applicant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.bnitest2.sasyadev.com/web/open/tokenator?concept=connect&amp;token=ejoZQWvsSSbsNAsbhKqSEAUTa9uO%2FE4XoiGFjGYWGniD76LGo6FTYCbUFuTC64EMAQyYzCremKISOb6%2Bpn0jfsFjZ5IG2DyL4pBOv8jvblAPgZbml6Qm4AqA09V60g7s3hCRuqG1oRBcwY3dJSSPigtFSI9D9rl6n4mTmwSjoJmkDsuHZ9jChw%3D%3D&amp;chapterId=816&amp;step=applicant</t>
   </si>
   <si>
     <t xml:space="preserve">brandNewVisitorEmailId</t>
@@ -38,6 +44,18 @@
     <t xml:space="preserve">lastName</t>
   </si>
   <si>
+    <t xml:space="preserve">dbselenium+v20200204124303@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selenium+v20200204124303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dbselenium+v20200204124646@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selenium+v20200204124646</t>
+  </si>
+  <si>
     <t xml:space="preserve">EmailID</t>
   </si>
   <si>
@@ -60,12 +78,6 @@
   </si>
   <si>
     <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t>https://www.bniconnectglobal.com/web/open/tokenator?concept=connect&amp;token=JFmUofFqkTdtuzjqYW3Oqtk5qlSHDIf3JMqw5JTU7r6yOU4bF4UPvaaNo2WZBuFBZBV3NCMLXdxSAnKi4wEZl%2FFIHJRdoxW%2BlY3Dw8XZjmSdbEzm1CwoGQ3JmPg75E1fA%2FRKb9vXdXo2lW2X2HEsGQsgh%2FfgoTyxvEOn4f3KyEc2MLy7zWUTpg%3D%3D&amp;chapterId=10927&amp;step=</t>
-  </si>
-  <si>
-    <t>https://www.bniconnectglobal.com/web/open/tokenator?concept=connect&amp;token=dl1fcOpOVIlwBRG70WYF%2FMbMZ183hNO3ylSHv6J0ADW4I0QFhvs7F9kXT%2BuD1SxAc%2FvQchHR9CjOYjdauFJwJgqT3bE3GH9PBOJSQo%2Bdqze4RYj5saST8kVkiOeLqyDCbQVf75YqkDzIn6jPVGw5zY7rfK05X6ZCD0f91n427Hs%3D&amp;chapterId=9406&amp;step=applicant</t>
   </si>
 </sst>
 </file>
@@ -164,7 +176,7 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -175,7 +187,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -194,9 +206,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -207,7 +219,17 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>12</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -241,10 +263,10 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -278,10 +300,10 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -315,7 +337,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -348,7 +370,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -380,7 +402,7 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -413,18 +435,18 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed minor defect in LaunchBrowser.java for chrome browser.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t xml:space="preserve">URL</t>
   </si>
@@ -78,6 +78,24 @@
   </si>
   <si>
     <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t>dbselenium+v20200204211239@gmail.com</t>
+  </si>
+  <si>
+    <t>selenium+v20200204211239</t>
+  </si>
+  <si>
+    <t>https://www.bnitest2.sasyadev.com/web/open/tokenator?concept=connect&amp;token=cQzzvAW7NGR1LDbnZCy95t%2FXLrJ5XPu83rMqH%2FkgAfXTEJtfi9OgWgbd0JIq%2BI3XHg87mKEqLKcLzbo8jZSnCK8sEvlvXa5lEPzTg8cxW2jWPGJqzdO3Mrto2KY7mQ8IvcQvkBIdUf8z1WWcRM7G%2F%2FuezrWLz7X3wlbgPOlxXLrt2Jl56ProgQ%3D%3D&amp;chapterId=816&amp;step=applicant</t>
+  </si>
+  <si>
+    <t>dbselenium+v20200213121448@gmail.com</t>
+  </si>
+  <si>
+    <t>selenium+v20200213121448</t>
+  </si>
+  <si>
+    <t>https://www.bnitest2.sasyadev.com/web/open/tokenator?concept=connect&amp;token=xMCwr0RoBRUpHSpIzcwMIj6oOcvftDDdBJkJwDjIK1%2BKErqvrr3hTf1z9KNylv5NRWwWYvmilW%2FZU%2BwMMzFq7vfki8M7rPEURI2SYLZtg%2FdX%2Fhkzoa%2FTcxIiH6nrScP%2B5skm1sivwpMNdKZn%2FINqgtJhCCv%2FeJ1ZEbYRaK6vBJDEDf9C5R2kPQ%3D%3D&amp;chapterId=816&amp;step=applicant</t>
   </si>
 </sst>
 </file>
@@ -206,7 +224,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -232,6 +250,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
@@ -248,7 +276,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -269,6 +297,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>

</xml_diff>

<commit_message>
Removed duplicate maven dependency for webdriverManager
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -276,7 +276,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -297,14 +297,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>

</xml_diff>